<commit_message>
Data for linear regresion
</commit_message>
<xml_diff>
--- a/experiments/20160427TestRegresion/test_regresioncarriersstat.xlsx
+++ b/experiments/20160427TestRegresion/test_regresioncarriersstat.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16828"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
     <sheet name="test_regresioncarriers" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -675,6 +675,990 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Regression </c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:yVal>
+            <c:numRef>
+              <c:f>test_regresioncarriers!$G$1:$G$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>18.900595753294951</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16.292181722717469</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16.028729848355617</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.716760720401929</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>35.33955689663955</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44.63234053372112</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>37.096380527578752</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>87.364715142993489</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>36.932348692994168</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>19.547221250770008</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>76.76988099745256</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>73.114042644204844</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>72.961353741464194</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>85.004265599733912</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>96.216868646391546</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>131.55528533178119</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>130.62256670126379</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>128.86775883405892</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>123.08173034322751</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>424.04604104117067</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>793.40937502978363</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D242-4D28-9EC3-4F0F78B968F9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Real Values</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:yVal>
+            <c:numRef>
+              <c:f>test_regresioncarriers!$C$1:$C$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>49.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>53.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>54.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>68.5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>72.5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>132.5</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>132.5</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>295</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>873</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-D242-4D28-9EC3-4F0F78B968F9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="334220216"/>
+        <c:axId val="334220544"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="334220216"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="334220544"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="334220544"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="334220216"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -974,10 +1958,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1229,6 +2213,12 @@
         <v>1001.4582909543959</v>
       </c>
     </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C24">
+        <f ca="1">C24</f>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1236,13 +2226,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O20" sqref="O20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>-0.428341567911111</v>
       </c>
@@ -1252,8 +2244,21 @@
       <c r="C1">
         <v>38</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="1">
+        <v>-1.79543372024074</v>
+      </c>
+      <c r="E1" s="2">
+        <v>893.94221744375545</v>
+      </c>
+      <c r="F1" s="1">
+        <v>16.061835565410419</v>
+      </c>
+      <c r="G1">
+        <f>A1*D1+B1*E1+F1</f>
+        <v>18.900595753294951</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1.1561049397858001</v>
       </c>
@@ -1263,8 +2268,21 @@
       <c r="C2">
         <v>37</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" s="1">
+        <v>-1.79543372024074</v>
+      </c>
+      <c r="E2" s="2">
+        <v>893.94221744375545</v>
+      </c>
+      <c r="F2" s="1">
+        <v>16.061835565410419</v>
+      </c>
+      <c r="G2">
+        <f t="shared" ref="G2:G21" si="0">A2*D2+B2*E2+F2</f>
+        <v>16.292181722717469</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1.26793873963718</v>
       </c>
@@ -1274,8 +2292,21 @@
       <c r="C3">
         <v>37</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" s="1">
+        <v>-1.79543372024074</v>
+      </c>
+      <c r="E3" s="2">
+        <v>893.94221744375545</v>
+      </c>
+      <c r="F3" s="1">
+        <v>16.061835565410419</v>
+      </c>
+      <c r="G3">
+        <f t="shared" si="0"/>
+        <v>16.028729848355617</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2.5636831354290099</v>
       </c>
@@ -1285,8 +2316,21 @@
       <c r="C4">
         <v>41</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" s="1">
+        <v>-1.79543372024074</v>
+      </c>
+      <c r="E4" s="2">
+        <v>893.94221744375545</v>
+      </c>
+      <c r="F4" s="1">
+        <v>16.061835565410419</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="0"/>
+        <v>16.716760720401929</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1.49232943784418</v>
       </c>
@@ -1296,8 +2340,21 @@
       <c r="C5">
         <v>49.5</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" s="1">
+        <v>-1.79543372024074</v>
+      </c>
+      <c r="E5" s="2">
+        <v>893.94221744375545</v>
+      </c>
+      <c r="F5" s="1">
+        <v>16.061835565410419</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>35.33955689663955</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1.1144230921335501</v>
       </c>
@@ -1307,8 +2364,21 @@
       <c r="C6">
         <v>50</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" s="1">
+        <v>-1.79543372024074</v>
+      </c>
+      <c r="E6" s="2">
+        <v>893.94221744375545</v>
+      </c>
+      <c r="F6" s="1">
+        <v>16.061835565410419</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>44.63234053372112</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>3.7604000172145802</v>
       </c>
@@ -1318,8 +2388,21 @@
       <c r="C7">
         <v>53.5</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" s="1">
+        <v>-1.79543372024074</v>
+      </c>
+      <c r="E7" s="2">
+        <v>893.94221744375545</v>
+      </c>
+      <c r="F7" s="1">
+        <v>16.061835565410419</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>37.096380527578752</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>-1.1963405020712901</v>
       </c>
@@ -1329,8 +2412,21 @@
       <c r="C8">
         <v>62</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" s="1">
+        <v>-1.79543372024074</v>
+      </c>
+      <c r="E8" s="2">
+        <v>893.94221744375545</v>
+      </c>
+      <c r="F8" s="1">
+        <v>16.061835565410419</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>87.364715142993489</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>3.8834896985960099</v>
       </c>
@@ -1340,8 +2436,21 @@
       <c r="C9">
         <v>54.5</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" s="1">
+        <v>-1.79543372024074</v>
+      </c>
+      <c r="E9" s="2">
+        <v>893.94221744375545</v>
+      </c>
+      <c r="F9" s="1">
+        <v>16.061835565410419</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>36.932348692994168</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>7.9620644227371402</v>
       </c>
@@ -1351,8 +2460,21 @@
       <c r="C10">
         <v>50</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" s="1">
+        <v>-1.79543372024074</v>
+      </c>
+      <c r="E10" s="2">
+        <v>893.94221744375545</v>
+      </c>
+      <c r="F10" s="1">
+        <v>16.061835565410419</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>19.547221250770008</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>5.4239692389862002</v>
       </c>
@@ -1362,8 +2484,21 @@
       <c r="C11">
         <v>70</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11" s="1">
+        <v>-1.79543372024074</v>
+      </c>
+      <c r="E11" s="2">
+        <v>893.94221744375545</v>
+      </c>
+      <c r="F11" s="1">
+        <v>16.061835565410419</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>76.76988099745256</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>6.7190087559729204</v>
       </c>
@@ -1373,8 +2508,21 @@
       <c r="C12">
         <v>68.5</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12" s="1">
+        <v>-1.79543372024074</v>
+      </c>
+      <c r="E12" s="2">
+        <v>893.94221744375545</v>
+      </c>
+      <c r="F12" s="1">
+        <v>16.061835565410419</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>73.114042644204844</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>8.3139798901207609</v>
       </c>
@@ -1384,8 +2532,21 @@
       <c r="C13">
         <v>72</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13" s="1">
+        <v>-1.79543372024074</v>
+      </c>
+      <c r="E13" s="2">
+        <v>893.94221744375545</v>
+      </c>
+      <c r="F13" s="1">
+        <v>16.061835565410419</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>72.961353741464194</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>8.5365924688430397</v>
       </c>
@@ -1395,8 +2556,21 @@
       <c r="C14">
         <v>72.5</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14" s="1">
+        <v>-1.79543372024074</v>
+      </c>
+      <c r="E14" s="2">
+        <v>893.94221744375545</v>
+      </c>
+      <c r="F14" s="1">
+        <v>16.061835565410419</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>85.004265599733912</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>8.39851216354249</v>
       </c>
@@ -1406,8 +2580,21 @@
       <c r="C15">
         <v>70</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15" s="1">
+        <v>-1.79543372024074</v>
+      </c>
+      <c r="E15" s="2">
+        <v>893.94221744375545</v>
+      </c>
+      <c r="F15" s="1">
+        <v>16.061835565410419</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="0"/>
+        <v>96.216868646391546</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>26.258695277001799</v>
       </c>
@@ -1417,8 +2604,21 @@
       <c r="C16">
         <v>110</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16" s="1">
+        <v>-1.79543372024074</v>
+      </c>
+      <c r="E16" s="2">
+        <v>893.94221744375545</v>
+      </c>
+      <c r="F16" s="1">
+        <v>16.061835565410419</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="0"/>
+        <v>131.55528533178119</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>26.5795606258948</v>
       </c>
@@ -1428,8 +2628,21 @@
       <c r="C17">
         <v>96</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17" s="1">
+        <v>-1.79543372024074</v>
+      </c>
+      <c r="E17" s="2">
+        <v>893.94221744375545</v>
+      </c>
+      <c r="F17" s="1">
+        <v>16.061835565410419</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="0"/>
+        <v>130.62256670126379</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>28.224151020964801</v>
       </c>
@@ -1439,8 +2652,21 @@
       <c r="C18">
         <v>132.5</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18" s="1">
+        <v>-1.79543372024074</v>
+      </c>
+      <c r="E18" s="2">
+        <v>893.94221744375545</v>
+      </c>
+      <c r="F18" s="1">
+        <v>16.061835565410419</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="0"/>
+        <v>128.86775883405892</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>30.733553816903999</v>
       </c>
@@ -1450,8 +2676,21 @@
       <c r="C19">
         <v>132.5</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19" s="1">
+        <v>-1.79543372024074</v>
+      </c>
+      <c r="E19" s="2">
+        <v>893.94221744375545</v>
+      </c>
+      <c r="F19" s="1">
+        <v>16.061835565410419</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="0"/>
+        <v>123.08173034322751</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>7.7556886912219403</v>
       </c>
@@ -1461,8 +2700,21 @@
       <c r="C20">
         <v>295</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20" s="1">
+        <v>-1.79543372024074</v>
+      </c>
+      <c r="E20" s="2">
+        <v>893.94221744375545</v>
+      </c>
+      <c r="F20" s="1">
+        <v>16.061835565410419</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="0"/>
+        <v>424.04604104117067</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>24.667932319572401</v>
       </c>
@@ -1471,10 +2723,24 @@
       </c>
       <c r="C21">
         <v>873</v>
+      </c>
+      <c r="D21" s="1">
+        <v>-1.79543372024074</v>
+      </c>
+      <c r="E21" s="2">
+        <v>893.94221744375545</v>
+      </c>
+      <c r="F21" s="1">
+        <v>16.061835565410419</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="0"/>
+        <v>793.40937502978363</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>